<commit_message>
images intégrées et disparition du formulaire via JV
</commit_message>
<xml_diff>
--- a/temps de travail eval2.xlsx
+++ b/temps de travail eval2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\volta\Documents\eval-studi\evaluation2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8B055F8-AFC7-4EA9-A9D4-66C944AB3379}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1615F14-6118-4D62-A84F-70446C314A69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{31F4BB13-8F26-47AF-A445-695FED4A5E1D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>jour</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>création des fichiers</t>
+  </si>
+  <si>
+    <t>mise en page statique</t>
   </si>
 </sst>
 </file>
@@ -396,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6106F0B2-35D9-4431-AFED-10C3D716BAD5}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,6 +426,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B3" s="2">
+        <v>5.9027777777777783E-2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout du fichier playing.js non fonctionnel
</commit_message>
<xml_diff>
--- a/temps de travail eval2.xlsx
+++ b/temps de travail eval2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\volta\Documents\eval-studi\evaluation2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1615F14-6118-4D62-A84F-70446C314A69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A865F58-82D4-43AD-B5FB-37C456E7EA73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{31F4BB13-8F26-47AF-A445-695FED4A5E1D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>jour</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>mise en page statique</t>
+  </si>
+  <si>
+    <t>apparence - modification affihchage JS</t>
   </si>
 </sst>
 </file>
@@ -399,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6106F0B2-35D9-4431-AFED-10C3D716BAD5}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,6 +440,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
le jeu fonctionne en console dans playing.js
</commit_message>
<xml_diff>
--- a/temps de travail eval2.xlsx
+++ b/temps de travail eval2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\volta\Documents\eval-studi\evaluation2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A865F58-82D4-43AD-B5FB-37C456E7EA73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492FB5CE-0DE2-4BFD-B089-17C486A8E16A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{31F4BB13-8F26-47AF-A445-695FED4A5E1D}"/>
+    <workbookView xWindow="1230" yWindow="3585" windowWidth="23970" windowHeight="6000" xr2:uid="{31F4BB13-8F26-47AF-A445-695FED4A5E1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>jour</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>apparence - modification affihchage JS</t>
+  </si>
+  <si>
+    <t>apprence - travail sur les avatars</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6106F0B2-35D9-4431-AFED-10C3D716BAD5}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,6 +454,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>44317</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout d'une jauge de score
</commit_message>
<xml_diff>
--- a/temps de travail eval2.xlsx
+++ b/temps de travail eval2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\volta\Documents\eval-studi\evaluation2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492FB5CE-0DE2-4BFD-B089-17C486A8E16A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72EE3BD-CF8C-471C-B84A-DC6E61C13569}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="3585" windowWidth="23970" windowHeight="6000" xr2:uid="{31F4BB13-8F26-47AF-A445-695FED4A5E1D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{31F4BB13-8F26-47AF-A445-695FED4A5E1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>jour</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>apprence - travail sur les avatars</t>
+  </si>
+  <si>
+    <t>fonctionnement du jeu</t>
   </si>
 </sst>
 </file>
@@ -405,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6106F0B2-35D9-4431-AFED-10C3D716BAD5}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,6 +468,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44318</v>
+      </c>
+      <c r="B6" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>